<commit_message>
Implementando el analisis final de la lista de requerimientos
</commit_message>
<xml_diff>
--- a/docs/SRS Evaluacion.xlsx
+++ b/docs/SRS Evaluacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Lenguaje_de_Programacion_Avanzado_1\Proyectos\lpa1-taller-evaluacion\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084264D3-DF28-48F1-8190-129A40D734B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF8B000-0769-4FA6-B71E-76CFF6B3F19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{D6272AEF-CFF1-420E-9E1E-EC385C6C2E53}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
   <si>
     <t>REQUERIMIENTOS FUNCIONALES</t>
   </si>
@@ -230,12 +230,75 @@
   <si>
     <t>OBSERVACIONES</t>
   </si>
+  <si>
+    <t>Posible redudancia con R3</t>
+  </si>
+  <si>
+    <t>No se especifica el publico al que ira dirigido las ofertas especiales, o solo seran para el hotel, ademas, puede haber conflicto con el R2</t>
+  </si>
+  <si>
+    <t>Falta informacion sobre como se relaciona con el R3</t>
+  </si>
+  <si>
+    <t>No especifica que pasarelas de pago necesita</t>
+  </si>
+  <si>
+    <t>No define las condiciones de cancelacion, ni tampoco que relacion tiene con el R16</t>
+  </si>
+  <si>
+    <t>No especifica de que manera se incorporan las politicas de cada hotel</t>
+  </si>
+  <si>
+    <t>No se especifica el formato de estas metricas ni tampoco el periodo de tiempo que usara para los reportes</t>
+  </si>
+  <si>
+    <t>No se especifica que caracteristicas tendra el administrador</t>
+  </si>
+  <si>
+    <t>Falta especificar como se implementara</t>
+  </si>
+  <si>
+    <t>No define que se entiende por escalable ni como se hara</t>
+  </si>
+  <si>
+    <t>No define tiempos de respuesta cuantilifables</t>
+  </si>
+  <si>
+    <t>No define que se entiende por interfaz intuitiva</t>
+  </si>
+  <si>
+    <t>No se mencionan que estandares en especifico se aplicaran</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>Posible redundancia con el R24</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +308,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -317,6 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,11 +406,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp100.xml><?xml version="1.0" encoding="utf-8"?>
@@ -347,7 +418,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
@@ -355,7 +426,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,11 +434,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp105.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp106.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp107.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,7 +454,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp110.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,7 +470,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp113.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp114.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,27 +478,27 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp115.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp116.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp117.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp118.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,7 +530,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp127.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp128.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,15 +538,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,23 +558,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -511,11 +582,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
@@ -523,39 +594,39 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
@@ -563,15 +634,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,15 +650,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
@@ -599,19 +670,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp43.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp44.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,15 +690,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -635,7 +706,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,135 +718,135 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp54.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp55.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp56.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp57.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp59.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp63.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp79.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
@@ -783,23 +854,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp87.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp88.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp89.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -807,7 +878,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp90.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp91.xml><?xml version="1.0" encoding="utf-8"?>
@@ -819,19 +890,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp93.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp94.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp95.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp96.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp97.xml><?xml version="1.0" encoding="utf-8"?>
@@ -839,11 +910,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp98.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp99.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8898,8 +8969,8 @@
           <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>238125</xdr:colOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>1295400</xdr:colOff>
           <xdr:row>74</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -9724,23 +9795,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F766C5C4-BCA0-4B39-ABEE-C2E0F61C2D01}">
-  <dimension ref="B2:H37"/>
+  <dimension ref="B2:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="121.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="122.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -9751,7 +9822,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -9773,8 +9844,9 @@
       <c r="H3" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -9785,9 +9857,12 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -9798,9 +9873,12 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -9811,9 +9889,11 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -9824,9 +9904,11 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -9837,9 +9919,11 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -9850,9 +9934,11 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -9863,9 +9949,11 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -9876,9 +9964,11 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
@@ -9889,9 +9979,11 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
@@ -9902,9 +9994,11 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
@@ -9915,9 +10009,11 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -9928,9 +10024,11 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
@@ -9941,7 +10039,9 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
@@ -9954,7 +10054,9 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
@@ -9967,7 +10069,9 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
@@ -9980,7 +10084,9 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
@@ -9993,7 +10099,9 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -10006,7 +10114,9 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
@@ -10019,7 +10129,9 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -10032,7 +10144,9 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
@@ -10045,7 +10159,9 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
@@ -10058,7 +10174,9 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
@@ -10071,7 +10189,9 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="H26" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -10084,7 +10204,9 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="28" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
@@ -10097,7 +10219,9 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
@@ -10135,7 +10259,7 @@
     </row>
     <row r="32" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>57</v>
@@ -10144,11 +10268,13 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>58</v>
@@ -10157,11 +10283,13 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="H33" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>59</v>
@@ -10170,11 +10298,13 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>60</v>
@@ -10183,11 +10313,13 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>61</v>
@@ -10196,11 +10328,13 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="37" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>62</v>
@@ -10209,7 +10343,9 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="H37" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12876,8 +13012,8 @@
                     <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>1295400</xdr:colOff>
                     <xdr:row>74</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </to>

</xml_diff>